<commit_message>
added old laptop code
</commit_message>
<xml_diff>
--- a/output/axis_sept_oct.xlsx
+++ b/output/axis_sept_oct.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Stock Name</t>
   </si>
@@ -24,1041 +24,6 @@
   </si>
   <si>
     <t>Variation</t>
-  </si>
-  <si>
-    <t>9.1% Dewan Housing Finance Corporation Limited NCD Ser IV (16/08/2019)</t>
-  </si>
-  <si>
-    <t>9.05% Dewan Housing Finance Corporation Limited NCD Ser I (09/09/2019)</t>
-  </si>
-  <si>
-    <t>Mahindra &amp; Mahindra Financial Services Limited (29/03/2022) (ZCB) **</t>
-  </si>
-  <si>
-    <t>9.60% Hindalco Industries Limited (02/08/2022) **</t>
-  </si>
-  <si>
-    <t>8.65% Housing Development Finance Corporation Limited (18/09/2020) **</t>
-  </si>
-  <si>
-    <t>9.21% Punjab National Bank (31/03/2022) **</t>
-  </si>
-  <si>
-    <t>8.57% REC Limited (21/12/2024) **</t>
-  </si>
-  <si>
-    <t>Bajaj Housing Finance Limited (05/04/2022) (ZCB) **</t>
-  </si>
-  <si>
-    <t>8.07% L&amp;T Finance Limited (29/05/2020) **</t>
-  </si>
-  <si>
-    <t>7.69% National Bank For Agriculture and Rural Development (31/03/2032) **</t>
-  </si>
-  <si>
-    <t>9.41% India Infrastructure Fin Co Ltd (27/07/2037) **</t>
-  </si>
-  <si>
-    <t>7.40% Housing Development Finance Corporation Limited (17/11/2020) **</t>
-  </si>
-  <si>
-    <t>8.32% Power Grid Corporation of India Limited (23/12/2020) **</t>
-  </si>
-  <si>
-    <t>7.14% REC Limited (09/12/2021) **</t>
-  </si>
-  <si>
-    <t>9.39% Power Finance Corporation Limited (27/08/2024) **</t>
-  </si>
-  <si>
-    <t>9.95% Syndicate Bank (25/10/2021) **</t>
-  </si>
-  <si>
-    <t>MFL Securitisation Trust (25/06/2021) ** #</t>
-  </si>
-  <si>
-    <t>9.15% Birla Corporation Limited (18/08/2021) **</t>
-  </si>
-  <si>
-    <t>11.00% PVR Limited (24/11/2019) **</t>
-  </si>
-  <si>
-    <t>8.58% Housing Development Finance Corporation Limited (18/03/2022)</t>
-  </si>
-  <si>
-    <t>7.07% Reliance Industries Limited (24/12/2020)</t>
-  </si>
-  <si>
-    <t>8.60% National Bank For Agriculture and Rural Development (31/01/2022) **</t>
-  </si>
-  <si>
-    <t>11.9414% Ess Kay Fincorp Limited (13/09/2022) **</t>
-  </si>
-  <si>
-    <t>8.15% Power Grid Corporation of India Limited (09/03/2020) **</t>
-  </si>
-  <si>
-    <t>8.37% National Bank For Agriculture and Rural Development (22/06/2020) **</t>
-  </si>
-  <si>
-    <t>8.20% Power Grid Corporation of India Limited (23/01/2030) **</t>
-  </si>
-  <si>
-    <t>7.39% LIC Housing Finance Limited (30/08/2022) **</t>
-  </si>
-  <si>
-    <t>6.80% Hindustan Petroleum Corporation Limited (15/12/2022)</t>
-  </si>
-  <si>
-    <t>7.42% LIC Housing Finance Limited (15/07/2022) **</t>
-  </si>
-  <si>
-    <t>9.02% REC Limited (19/11/2022) **</t>
-  </si>
-  <si>
-    <t>8.56% REC Limited (29/11/2028) **</t>
-  </si>
-  <si>
-    <t>9.10% Union Bank of India (31/03/2022) **</t>
-  </si>
-  <si>
-    <t>8.53% Power Finance Corporation Limited (24/07/2020)</t>
-  </si>
-  <si>
-    <t>9.20% ICICI Bank Limited (17/03/2022) **</t>
-  </si>
-  <si>
-    <t>Cholamandalam Investment and Finance Company Limited (29/04/2020) (ZCB) **</t>
-  </si>
-  <si>
-    <t>1.5% Housing Development Finance Corporation Limited (30/03/2020) **</t>
-  </si>
-  <si>
-    <t>JM Financial Products  Limited (13/09/2021) (ZCB) **</t>
-  </si>
-  <si>
-    <t>11.25% Hansdeep Industries &amp; Trading Company Limited (28/09/2020) **</t>
-  </si>
-  <si>
-    <t>7.05% Power Finance Corporation Limited (15/05/2020) **</t>
-  </si>
-  <si>
-    <t>7.84% PVR Limited (10/07/2020) **</t>
-  </si>
-  <si>
-    <t>8.80% REC Limited (29/11/2020) **</t>
-  </si>
-  <si>
-    <t>11.4321% Asirvad Microfinance Ltd (22/06/2020) **</t>
-  </si>
-  <si>
-    <t>7.40% Jamnagar Utilities &amp; Power Private Limited (29/07/2020) **</t>
-  </si>
-  <si>
-    <t>8.83% REC Limited (21/01/2022) **</t>
-  </si>
-  <si>
-    <t>8.50% LIC Housing Finance Limited (20/06/2022) **</t>
-  </si>
-  <si>
-    <t>8.76% Power Finance Corporation Limited (07/11/2019) **</t>
-  </si>
-  <si>
-    <t>8.32% Reliance Jio Infocomm Limited (08/07/2021) **</t>
-  </si>
-  <si>
-    <t>8.05% Housing Development Finance Corporation Limited (20/06/2022) **</t>
-  </si>
-  <si>
-    <t>National Bank For Agriculture and Rural Development (13/03/2020) #</t>
-  </si>
-  <si>
-    <t>7.33% Jamnagar Utilities &amp; Power Private Limited (28/02/2020) **</t>
-  </si>
-  <si>
-    <t>9.11% Housing Development Finance Corporation Limited (13/12/2019) **</t>
-  </si>
-  <si>
-    <t>JSW Techno Projects Management Limited (28/02/2020) (ZCB) ** #</t>
-  </si>
-  <si>
-    <t>9.39% Aditya Birla Finance Limited (29/04/2020) **</t>
-  </si>
-  <si>
-    <t>7.13% REC Limited (21/09/2020)</t>
-  </si>
-  <si>
-    <t>8.45% Shriram Transport Finance Company Limited (27/03/2020) **</t>
-  </si>
-  <si>
-    <t>9.48% REC Limited (10/08/2021) **</t>
-  </si>
-  <si>
-    <t>8.50% Bank of Baroda (02/12/2021) **</t>
-  </si>
-  <si>
-    <t>7.89% Small Industries Dev Bank of India (15/11/2022) **</t>
-  </si>
-  <si>
-    <t>8.38% Power Finance Corporation Limited (27/04/2020) **</t>
-  </si>
-  <si>
-    <t>6.98% National Bank For Agriculture and Rural Development (19/09/2022)</t>
-  </si>
-  <si>
-    <t>9.15% ICICI Bank Limited (20/06/2023) **</t>
-  </si>
-  <si>
-    <t>MFL Securitisation Trust (15/09/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.25% Bharti Airtel Limited (20/04/2020) **</t>
-  </si>
-  <si>
-    <t>8.70% Power Finance Corporation Limited (15/07/2020) **</t>
-  </si>
-  <si>
-    <t>9.48% Bank of Baroda (09/01/2020) **</t>
-  </si>
-  <si>
-    <t>Britannia Industries Limited</t>
-  </si>
-  <si>
-    <t>Dr. Reddy's Laboratories Limited</t>
-  </si>
-  <si>
-    <t>8.8228% Shriram Transport Finance Company Limited (27/04/2020) **</t>
-  </si>
-  <si>
-    <t>11.955% Northern Arc Capital Limited (25/06/2021) **</t>
-  </si>
-  <si>
-    <t>MFL Securitisation Trust (15/04/2020) ** #</t>
-  </si>
-  <si>
-    <t>9.08% Union Bank of India (03/05/2022) **</t>
-  </si>
-  <si>
-    <t>7.99% Tata Power Company Limited (16/11/2021) **</t>
-  </si>
-  <si>
-    <t>7.60% Hero Fincorp Limited (18/11/2020) **</t>
-  </si>
-  <si>
-    <t>8.37% REC Limited (07/12/2028) **</t>
-  </si>
-  <si>
-    <t>8.95% Punjab National Bank (03/03/2022) **</t>
-  </si>
-  <si>
-    <t>7.15% Housing Development Finance Corporation Limited (16/09/2021) **</t>
-  </si>
-  <si>
-    <t>7.32% NTPC Limited (17/07/2029) **</t>
-  </si>
-  <si>
-    <t>9.00% Talwandi Sabo Power Limited (30/11/2020) **</t>
-  </si>
-  <si>
-    <t>LIC Housing Finance Limited (25/02/2020) (ZCB) **</t>
-  </si>
-  <si>
-    <t>7.50% Power Finance Corporation Limited (16/08/2021) **</t>
-  </si>
-  <si>
-    <t>8.00% Reliance Jio Infocomm Limited (07/04/2023) **</t>
-  </si>
-  <si>
-    <t>8.15% REC Limited (18/06/2021) **</t>
-  </si>
-  <si>
-    <t>7.90% Tata Sons Private Ltd (06/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.42% Bank of Baroda (07/12/2028) **</t>
-  </si>
-  <si>
-    <t>8.95% Reliance Jio Infocomm Limited (18/11/2019) **</t>
-  </si>
-  <si>
-    <t>7.18% National Bank For Agriculture and Rural Development (08/08/2022)</t>
-  </si>
-  <si>
-    <t>7.17% Reliance Industries Limited (08/11/2022) **</t>
-  </si>
-  <si>
-    <t>7.73% REC Limited (15/06/2021) **</t>
-  </si>
-  <si>
-    <t>9.02% LIC Housing Finance Limited (03/12/2020) **</t>
-  </si>
-  <si>
-    <t>7.92% Hero Fincorp Limited (05/06/2020) **</t>
-  </si>
-  <si>
-    <t>8.7% JK Lakshmi Cement Limited (06/01/2020) **</t>
-  </si>
-  <si>
-    <t>6.98% National Bank For Agriculture and Rural Development (30/09/2020) **</t>
-  </si>
-  <si>
-    <t>8.75% Indiabulls Housing Finance Limited (21/02/2020) **</t>
-  </si>
-  <si>
-    <t>Reliable Devices Trust (21/12/2020) **</t>
-  </si>
-  <si>
-    <t>11.25% Hansdeep Industries &amp; Trading Company Limited (13/08/2020) **</t>
-  </si>
-  <si>
-    <t>Aditya Birla Finance Limited (05/06/2020) (ZCB) **</t>
-  </si>
-  <si>
-    <t>7.9803% Mahindra &amp; Mahindra Financial Services Limited (13/03/2020) **</t>
-  </si>
-  <si>
-    <t>7.99% LIC Housing Finance Limited (12/07/2029) **</t>
-  </si>
-  <si>
-    <t>7.74% LIC Housing Finance Limited (05/06/2020) **</t>
-  </si>
-  <si>
-    <t>9.8762% IndoStar Capital Finance Limited (01/11/2019) **</t>
-  </si>
-  <si>
-    <t>9.15% Coastal Gujarat Power Limited (14/06/2021) **</t>
-  </si>
-  <si>
-    <t>8.64% IDFC First Bank Limited (15/04/2020) **</t>
-  </si>
-  <si>
-    <t>6.80% National Bank For Agriculture and Rural Development (03/03/2020) **</t>
-  </si>
-  <si>
-    <t>7.47% Power Finance Corporation Limited (16/09/2021) **</t>
-  </si>
-  <si>
-    <t>Rainbow Devices Trust (28/09/2020) **</t>
-  </si>
-  <si>
-    <t>7.00% Reliance Industries Limited (31/08/2022)</t>
-  </si>
-  <si>
-    <t>9.15% Essel Mining And Industries Ltd (17/07/2022) ** #</t>
-  </si>
-  <si>
-    <t>Orelia Trust Aug 2019 (24/08/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.50% National Bank For Agriculture and Rural Development (31/01/2022) **</t>
-  </si>
-  <si>
-    <t>9.85% Adani Transmission Limited (16/12/2019) **</t>
-  </si>
-  <si>
-    <t>8.10% Power Finance Corporation Limited (04/06/2024) **</t>
-  </si>
-  <si>
-    <t>7.70% National Highways Auth Of Ind (13/09/2029)</t>
-  </si>
-  <si>
-    <t>8.65% Dalmia Cement (Bharat) Limited (19/10/2020) **</t>
-  </si>
-  <si>
-    <t>9.15% Coastal Gujarat Power Limited (12/06/2020) **</t>
-  </si>
-  <si>
-    <t>TMF Holdings Limited (24/01/2020) (ZCB) ** #</t>
-  </si>
-  <si>
-    <t>RENT-A-DEVICE TRUST (28/09/2020) **</t>
-  </si>
-  <si>
-    <t>10.35% Bahadur Chand Investments Pvt Limited (16/01/2024) ** #</t>
-  </si>
-  <si>
-    <t>8.36% Power Finance Corporation Limited (04/09/2020) **</t>
-  </si>
-  <si>
-    <t>8.68% Grasim Industries Limited (02/02/2020) **</t>
-  </si>
-  <si>
-    <t>Bahadur Chand Investments Pvt Limited (28/01/2020) #</t>
-  </si>
-  <si>
-    <t>Reliance Industries Limited (03/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>JM Financial Products  Limited (24/12/2019) ** #</t>
-  </si>
-  <si>
-    <t>8.70% Housing Development Finance Corporation Limited (15/12/2020)</t>
-  </si>
-  <si>
-    <t>8.40% Dewan Housing Finance Corporation Limited (27/12/2019) ^</t>
-  </si>
-  <si>
-    <t>6.95% Reliance Industries Limited (14/12/2020)</t>
-  </si>
-  <si>
-    <t>8.05% National Housing Bank (10/01/2022) **</t>
-  </si>
-  <si>
-    <t>RELIANCE RETAIL LTD (16/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>7.65% National Housing Bank (25/03/2022) **</t>
-  </si>
-  <si>
-    <t>9.6556% Tata Motors Finance Limited (20/03/2020) **</t>
-  </si>
-  <si>
-    <t>Kotak Mahindra Prime Limited (17/01/2020) ** #</t>
-  </si>
-  <si>
-    <t>Barclays Investments &amp; Loans (India) Private Limited (28/02/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.90% Reliance Jio Infocomm Limited (21/01/2020) **</t>
-  </si>
-  <si>
-    <t>9.0291% Tata Motors Finance Limited (30/01/2020) **</t>
-  </si>
-  <si>
-    <t>8.20% Power Finance Corporation Limited (14/09/2020) **</t>
-  </si>
-  <si>
-    <t>8.15% National Bank For Agriculture and Rural Development (22/08/2022) **</t>
-  </si>
-  <si>
-    <t>7.24% LIC Housing Finance Limited (23/08/2021) **</t>
-  </si>
-  <si>
-    <t>8.595% LIC Housing Finance Limited (14/01/2022) **</t>
-  </si>
-  <si>
-    <t>6.77% Larsen &amp; Toubro Limited (20/08/2020) **</t>
-  </si>
-  <si>
-    <t>Housing Development Finance Corporation Limited (26/05/2020) ** #</t>
-  </si>
-  <si>
-    <t>National Bank For Agriculture and Rural Development (15/05/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.36% Power Finance Corporation Limited (26/02/2020) **</t>
-  </si>
-  <si>
-    <t>Zee Entertainment Enterprises Limited</t>
-  </si>
-  <si>
-    <t>HSBC InvestDirect Financial Services (India) Limited (10/02/2020) ** #</t>
-  </si>
-  <si>
-    <t>Larsen &amp; Toubro Limited (27/12/2019) ** #</t>
-  </si>
-  <si>
-    <t>Britannia Industries Limited (20/12/2019) ** #</t>
-  </si>
-  <si>
-    <t>Kotak Mahindra Bank Limited (15/11/2019) ** #</t>
-  </si>
-  <si>
-    <t>Cholamandalam Investment and Finance Company Limited (12/06/2020) ** #</t>
-  </si>
-  <si>
-    <t>Kotak Mahindra Prime Limited (28/09/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.50% National Bank For Agriculture and Rural Development (31/01/2023)</t>
-  </si>
-  <si>
-    <t>Reliance Industries Limited (02/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.28% Oriental Nagpur Betul Highway Limited (30/09/2022) **</t>
-  </si>
-  <si>
-    <t>7.90% Nirma Limited (28/02/2020) **</t>
-  </si>
-  <si>
-    <t>Bharti Infratel Limited</t>
-  </si>
-  <si>
-    <t>Larsen &amp; Toubro Limited (28/02/2020) ** #</t>
-  </si>
-  <si>
-    <t>National Bank For Agriculture and Rural Development (18/02/2020) ** #</t>
-  </si>
-  <si>
-    <t>IndusInd Bank Limited (11/11/2019) #</t>
-  </si>
-  <si>
-    <t>Shriram Transport Finance Company Limited</t>
-  </si>
-  <si>
-    <t>ICICI Bank Limited (25/11/2019) ** #</t>
-  </si>
-  <si>
-    <t>Emami Limited (16/12/2019) ** #</t>
-  </si>
-  <si>
-    <t>Wipro Limited</t>
-  </si>
-  <si>
-    <t>ICICI Bank Limited (23/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>IDFC First Bank Limited (11/12/2019) ** #</t>
-  </si>
-  <si>
-    <t>Bank of Baroda (01/06/2020) #</t>
-  </si>
-  <si>
-    <t>8.28% Oriental Nagpur Betul Highway Limited (30/03/2020) **</t>
-  </si>
-  <si>
-    <t>Coal India Limited</t>
-  </si>
-  <si>
-    <t>Axis Bank Limited</t>
-  </si>
-  <si>
-    <t>Yes Bank Limited</t>
-  </si>
-  <si>
-    <t>Godrej Properties Limited</t>
-  </si>
-  <si>
-    <t>Indian Oil Corporation Limited</t>
-  </si>
-  <si>
-    <t>Oil &amp; Natural Gas Corporation Limited</t>
-  </si>
-  <si>
-    <t>Blue Dart Express Limited</t>
-  </si>
-  <si>
-    <t>9.10% Shriram Transport Finance Company Limited (12/07/2021) **</t>
-  </si>
-  <si>
-    <t>Bank of Baroda (02/04/2020) ** #</t>
-  </si>
-  <si>
-    <t>National Bank For Agriculture and Rural Development (16/07/2020) ** #</t>
-  </si>
-  <si>
-    <t>IndusInd Bank Limited (26/02/2020) ** #</t>
-  </si>
-  <si>
-    <t>IDFC First Bank Limited (26/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>Tata Global Beverages Limited</t>
-  </si>
-  <si>
-    <t>Bharat Petroleum Corporation Limited</t>
-  </si>
-  <si>
-    <t>NTPC Limited</t>
-  </si>
-  <si>
-    <t>Exide Industries Limited</t>
-  </si>
-  <si>
-    <t>Grasim Industries Limited</t>
-  </si>
-  <si>
-    <t>National Bank For Agriculture and Rural Development (06/03/2020) ** #</t>
-  </si>
-  <si>
-    <t>8.12% Government of India (10/12/2020)</t>
-  </si>
-  <si>
-    <t>Glenmark Pharmaceuticals Limited</t>
-  </si>
-  <si>
-    <t>Power Finance Corporation Limited</t>
-  </si>
-  <si>
-    <t>Small Industries Dev Bank of India (03/04/2020) ** #</t>
-  </si>
-  <si>
-    <t>MRF Limited</t>
-  </si>
-  <si>
-    <t>Adani Ports and Special Economic Zone Limited</t>
-  </si>
-  <si>
-    <t>The Federal Bank  Limited</t>
-  </si>
-  <si>
-    <t>8.35% Government of India (14/05/2022)</t>
-  </si>
-  <si>
-    <t>Equitas Holdings Limited</t>
-  </si>
-  <si>
-    <t>Bajaj Auto Limited</t>
-  </si>
-  <si>
-    <t>Tata Chemicals Limited</t>
-  </si>
-  <si>
-    <t>Arti Surfactants Limited ** #</t>
-  </si>
-  <si>
-    <t>Lupin Limited</t>
-  </si>
-  <si>
-    <t>L&amp;T Finance Holdings Limited</t>
-  </si>
-  <si>
-    <t>Schaeffler India Limited</t>
-  </si>
-  <si>
-    <t>IndusInd Bank Limited</t>
-  </si>
-  <si>
-    <t>Cadila Healthcare Limited</t>
-  </si>
-  <si>
-    <t>Tata Power Company Limited</t>
-  </si>
-  <si>
-    <t>Marico Limited</t>
-  </si>
-  <si>
-    <t>DLF Limited</t>
-  </si>
-  <si>
-    <t>Indiamart Intermesh Limited</t>
-  </si>
-  <si>
-    <t>Arti Surfactants Limited **</t>
-  </si>
-  <si>
-    <t>State Bank of India</t>
-  </si>
-  <si>
-    <t>7.72% Government of India (26/10/2055)</t>
-  </si>
-  <si>
-    <t>UPL Limited</t>
-  </si>
-  <si>
-    <t>Hindalco Industries Limited</t>
-  </si>
-  <si>
-    <t>LIC Housing Finance Limited</t>
-  </si>
-  <si>
-    <t>7.59% Government of India (11/01/2026)</t>
-  </si>
-  <si>
-    <t>Power Grid Corporation of India Limited</t>
-  </si>
-  <si>
-    <t>NMDC Limited</t>
-  </si>
-  <si>
-    <t>VST Industries Limited</t>
-  </si>
-  <si>
-    <t>MM Forgings Limited</t>
-  </si>
-  <si>
-    <t>Alkem Laboratories Limited</t>
-  </si>
-  <si>
-    <t>Sanofi India Limited</t>
-  </si>
-  <si>
-    <t>Minda Industries Limited</t>
-  </si>
-  <si>
-    <t>GAIL (India) Limited</t>
-  </si>
-  <si>
-    <t>Ambuja Cements Limited</t>
-  </si>
-  <si>
-    <t>Vinati Organics Limited</t>
-  </si>
-  <si>
-    <t>Torrent Pharmaceuticals Limited</t>
-  </si>
-  <si>
-    <t>PNC Infratech Limited</t>
-  </si>
-  <si>
-    <t>Eicher Motors Limited</t>
-  </si>
-  <si>
-    <t>Tata Steel Limited</t>
-  </si>
-  <si>
-    <t>Shree Cement Limited</t>
-  </si>
-  <si>
-    <t>Axis Gold ETF</t>
-  </si>
-  <si>
-    <t>JSW Steel Limited</t>
-  </si>
-  <si>
-    <t>Indian Railway Catering And Tourism Corporation Limited</t>
-  </si>
-  <si>
-    <t>JK Lakshmi Cement Limited</t>
-  </si>
-  <si>
-    <t>Larsen &amp; Toubro Infotech Limited</t>
-  </si>
-  <si>
-    <t>9.00% Muthoot Finance Limited (30/01/2020) **</t>
-  </si>
-  <si>
-    <t>Tata Motors Limited</t>
-  </si>
-  <si>
-    <t>Dabur India Limited</t>
-  </si>
-  <si>
-    <t>HCL Technologies Limited</t>
-  </si>
-  <si>
-    <t>Hero MotoCorp Limited</t>
-  </si>
-  <si>
-    <t>AIA Engineering Limited</t>
-  </si>
-  <si>
-    <t>Grindwell Norton Limited</t>
-  </si>
-  <si>
-    <t>8.75% Muthoot Finance Limited (19/06/2021) **</t>
-  </si>
-  <si>
-    <t>Vesuvius India Limited</t>
-  </si>
-  <si>
-    <t>Whirlpool of India Limited</t>
-  </si>
-  <si>
-    <t>SKF India Limited</t>
-  </si>
-  <si>
-    <t>8.75% Muthoot Finance Limited (24/06/2020) **</t>
-  </si>
-  <si>
-    <t>9.5% Blue Dart Express Limited (20/11/2019) **</t>
-  </si>
-  <si>
-    <t>HDFC Life Insurance Company Limited</t>
-  </si>
-  <si>
-    <t>SRF Limited</t>
-  </si>
-  <si>
-    <t>Blue Star Limited</t>
-  </si>
-  <si>
-    <t>Aurobindo Pharma Limited</t>
-  </si>
-  <si>
-    <t>Fine Organic Industries Limited</t>
-  </si>
-  <si>
-    <t>TTK Healthcare Limited</t>
-  </si>
-  <si>
-    <t>Cipla Limited</t>
-  </si>
-  <si>
-    <t>United Breweries Limited</t>
-  </si>
-  <si>
-    <t>Container Corporation of India Limited</t>
-  </si>
-  <si>
-    <t>Cholamandalam Financial Holdings Limited</t>
-  </si>
-  <si>
-    <t>Igarashi Motors India Limited</t>
-  </si>
-  <si>
-    <t>8.06% State Government Securities (27/03/2029)</t>
-  </si>
-  <si>
-    <t>8.28% Government of India (21/09/2027)</t>
-  </si>
-  <si>
-    <t>Gulf Oil Lubricants India Limited</t>
-  </si>
-  <si>
-    <t>TVS Motor Company Limited</t>
-  </si>
-  <si>
-    <t>Galaxy Surfactants Limited</t>
-  </si>
-  <si>
-    <t>Syngene International Limited</t>
-  </si>
-  <si>
-    <t>KNR Constructions Limited</t>
-  </si>
-  <si>
-    <t>AU Small Finance Bank Limited</t>
-  </si>
-  <si>
-    <t>Jindal Steel &amp; Power Limited</t>
-  </si>
-  <si>
-    <t>UltraTech Cement Limited</t>
-  </si>
-  <si>
-    <t>JK Cement Limited</t>
-  </si>
-  <si>
-    <t>Max Financial Services Limited</t>
-  </si>
-  <si>
-    <t>WABCO India Limited</t>
-  </si>
-  <si>
-    <t>NIIT Technologies Limited</t>
-  </si>
-  <si>
-    <t>Chalet Hotels Limited</t>
-  </si>
-  <si>
-    <t>United Spirits Limited</t>
-  </si>
-  <si>
-    <t>Balkrishna Industries Limited</t>
-  </si>
-  <si>
-    <t>Ahluwalia Contracts (India) Limited</t>
-  </si>
-  <si>
-    <t>364 Days Tbill (MD 26/12/2019)</t>
-  </si>
-  <si>
-    <t>Nestle India Limited</t>
-  </si>
-  <si>
-    <t>Bata India Limited</t>
-  </si>
-  <si>
-    <t>Coromandel International Limited</t>
-  </si>
-  <si>
-    <t>Neogen Chemicals Limited</t>
-  </si>
-  <si>
-    <t>Orient Refractories Limited</t>
-  </si>
-  <si>
-    <t>Dish TV India Limited</t>
-  </si>
-  <si>
-    <t>Punjab National Bank</t>
-  </si>
-  <si>
-    <t>MphasiS Limited</t>
-  </si>
-  <si>
-    <t>TTK Prestige Limited</t>
-  </si>
-  <si>
-    <t>IPCA Laboratories Limited</t>
-  </si>
-  <si>
-    <t>Can Fin Homes Limited</t>
-  </si>
-  <si>
-    <t>Orient Electric Limited</t>
-  </si>
-  <si>
-    <t>Kansai Nerolac Paints Limited</t>
-  </si>
-  <si>
-    <t>Brigade Enterprises Limited</t>
-  </si>
-  <si>
-    <t>Bajaj Finserv Limited</t>
-  </si>
-  <si>
-    <t>ACC Limited</t>
-  </si>
-  <si>
-    <t>PI Industries Limited</t>
-  </si>
-  <si>
-    <t>Trent Limited</t>
-  </si>
-  <si>
-    <t>TCNS Clothing Co. Limited</t>
-  </si>
-  <si>
-    <t>Sundaram Finance Holdings Limited</t>
-  </si>
-  <si>
-    <t>Bank of Baroda</t>
-  </si>
-  <si>
-    <t>Multi Commodity Exchange of India Limited</t>
-  </si>
-  <si>
-    <t>Varroc Engineering Limited</t>
-  </si>
-  <si>
-    <t>JM Financial Limited</t>
-  </si>
-  <si>
-    <t>Sun Pharmaceutical Industries Limited</t>
-  </si>
-  <si>
-    <t>Petronet LNG Limited</t>
-  </si>
-  <si>
-    <t>Vedanta Limited</t>
-  </si>
-  <si>
-    <t>Camlin Fine Sciences Limited</t>
-  </si>
-  <si>
-    <t>Adani Power Limited</t>
-  </si>
-  <si>
-    <t>ITC Limited</t>
-  </si>
-  <si>
-    <t>Aarti Industries Limited</t>
-  </si>
-  <si>
-    <t>Mahindra &amp; Mahindra Limited</t>
-  </si>
-  <si>
-    <t>Maruti Suzuki India Limited</t>
-  </si>
-  <si>
-    <t>Titan Company Limited</t>
-  </si>
-  <si>
-    <t>Bharti Airtel Limited</t>
-  </si>
-  <si>
-    <t>Mas Financial Services Limited</t>
-  </si>
-  <si>
-    <t>Indraprastha Gas Limited</t>
-  </si>
-  <si>
-    <t>HeidelbergCement India Limited</t>
-  </si>
-  <si>
-    <t>Hindustan Unilever Limited</t>
-  </si>
-  <si>
-    <t>Voltas Limited</t>
-  </si>
-  <si>
-    <t>Ashok Leyland Limited</t>
-  </si>
-  <si>
-    <t>Symphony Limited</t>
-  </si>
-  <si>
-    <t>Berger Paints (I) Limited</t>
-  </si>
-  <si>
-    <t>Sundaram Finance Limited</t>
-  </si>
-  <si>
-    <t>Endurance Technologies Limited</t>
-  </si>
-  <si>
-    <t>Supreme Industries Limited</t>
-  </si>
-  <si>
-    <t>The Indian Hotels Company Limited</t>
-  </si>
-  <si>
-    <t>Aditya Birla Fashion and Retail Limited</t>
-  </si>
-  <si>
-    <t>Divi's Laboratories Limited</t>
-  </si>
-  <si>
-    <t>Astral Poly Technik Limited</t>
-  </si>
-  <si>
-    <t>Tech Mahindra Limited</t>
-  </si>
-  <si>
-    <t>Larsen &amp; Toubro Limited</t>
-  </si>
-  <si>
-    <t>Asian Paints Limited</t>
-  </si>
-  <si>
-    <t>Mahindra &amp; Mahindra Financial Services Limited</t>
-  </si>
-  <si>
-    <t>Info Edge (India) Limited</t>
-  </si>
-  <si>
-    <t>Cholamandalam Investment and Finance Company Limited</t>
-  </si>
-  <si>
-    <t>Bajaj Finance Limited</t>
-  </si>
-  <si>
-    <t>Cummins India Limited</t>
-  </si>
-  <si>
-    <t>Housing Development Finance Corporation Limited</t>
-  </si>
-  <si>
-    <t>Infosys Limited</t>
-  </si>
-  <si>
-    <t>Reliance Industries Limited</t>
-  </si>
-  <si>
-    <t>Pidilite Industries Limited</t>
-  </si>
-  <si>
-    <t>Tata Consultancy Services Limited</t>
-  </si>
-  <si>
-    <t>Avenue Supermarts Limited</t>
-  </si>
-  <si>
-    <t>V-Guard Industries Limited</t>
-  </si>
-  <si>
-    <t>City Union Bank Limited</t>
-  </si>
-  <si>
-    <t>Kotak Mahindra Bank Limited</t>
-  </si>
-  <si>
-    <t>Torrent Power Limited</t>
-  </si>
-  <si>
-    <t>HDFC Bank Limited</t>
-  </si>
-  <si>
-    <t>Motherson Sumi Systems Limited</t>
-  </si>
-  <si>
-    <t>Bandhan Bank Limited</t>
-  </si>
-  <si>
-    <t>ICICI Bank Limited</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +81,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="73.9765625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="15.203125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="22.26953125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="17.578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.53125" customWidth="true" bestFit="true"/>
@@ -1137,9 +102,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2"/>
       <c r="B2" t="n">
         <v>0.009490421369931553</v>
       </c>
@@ -1151,9 +114,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3"/>
       <c r="B3" t="n">
         <v>0.01804098226688211</v>
       </c>
@@ -1165,9 +126,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4"/>
       <c r="B4" t="n">
         <v>4.0</v>
       </c>
@@ -1179,9 +138,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5"/>
       <c r="B5" t="n">
         <v>5.0</v>
       </c>
@@ -1193,9 +150,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6"/>
       <c r="B6" t="n">
         <v>5.0</v>
       </c>
@@ -1207,9 +162,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7"/>
       <c r="B7" t="n">
         <v>10.0</v>
       </c>
@@ -1221,9 +174,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8"/>
       <c r="B8" t="n">
         <v>10.0</v>
       </c>
@@ -1235,9 +186,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9"/>
       <c r="B9" t="n">
         <v>14.0</v>
       </c>
@@ -1249,9 +198,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10"/>
       <c r="B10" t="n">
         <v>15.0</v>
       </c>
@@ -1263,9 +210,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
+      <c r="A11"/>
       <c r="B11" t="n">
         <v>20.0</v>
       </c>
@@ -1277,9 +222,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
+      <c r="A12"/>
       <c r="B12" t="n">
         <v>25.0</v>
       </c>
@@ -1291,9 +234,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
+      <c r="A13"/>
       <c r="B13" t="n">
         <v>0.0</v>
       </c>
@@ -1305,9 +246,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
+      <c r="A14"/>
       <c r="B14" t="n">
         <v>30.0</v>
       </c>
@@ -1319,9 +258,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
+      <c r="A15"/>
       <c r="B15" t="n">
         <v>30.0</v>
       </c>
@@ -1333,9 +270,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
+      <c r="A16"/>
       <c r="B16" t="n">
         <v>35.0</v>
       </c>
@@ -1347,9 +282,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
+      <c r="A17"/>
       <c r="B17" t="n">
         <v>40.0</v>
       </c>
@@ -1361,9 +294,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
+      <c r="A18"/>
       <c r="B18" t="n">
         <v>48.0</v>
       </c>
@@ -1375,9 +306,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
+      <c r="A19"/>
       <c r="B19" t="n">
         <v>49.0</v>
       </c>
@@ -1389,9 +318,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
+      <c r="A20"/>
       <c r="B20" t="n">
         <v>50.0</v>
       </c>
@@ -1403,9 +330,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
+      <c r="A21"/>
       <c r="B21" t="n">
         <v>0.0</v>
       </c>
@@ -1417,9 +342,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
+      <c r="A22"/>
       <c r="B22" t="n">
         <v>0.0</v>
       </c>
@@ -1431,9 +354,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
+      <c r="A23"/>
       <c r="B23" t="n">
         <v>50.0</v>
       </c>
@@ -1445,9 +366,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
+      <c r="A24"/>
       <c r="B24" t="n">
         <v>50.0</v>
       </c>
@@ -1459,9 +378,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
+      <c r="A25"/>
       <c r="B25" t="n">
         <v>50.0</v>
       </c>
@@ -1473,9 +390,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
+      <c r="A26"/>
       <c r="B26" t="n">
         <v>80.0</v>
       </c>
@@ -1487,9 +402,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
+      <c r="A27"/>
       <c r="B27" t="n">
         <v>50.0</v>
       </c>
@@ -1501,9 +414,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
+      <c r="A28"/>
       <c r="B28" t="n">
         <v>0.0</v>
       </c>
@@ -1515,9 +426,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
+      <c r="A29"/>
       <c r="B29" t="n">
         <v>0.0</v>
       </c>
@@ -1529,9 +438,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
+      <c r="A30"/>
       <c r="B30" t="n">
         <v>0.0</v>
       </c>
@@ -1543,9 +450,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
+      <c r="A31"/>
       <c r="B31" t="n">
         <v>0.0</v>
       </c>
@@ -1557,9 +462,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
+      <c r="A32"/>
       <c r="B32" t="n">
         <v>50.0</v>
       </c>
@@ -1571,9 +474,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
+      <c r="A33"/>
       <c r="B33" t="n">
         <v>50.0</v>
       </c>
@@ -1585,9 +486,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
+      <c r="A34"/>
       <c r="B34" t="n">
         <v>0.0</v>
       </c>
@@ -1599,9 +498,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
+      <c r="A35"/>
       <c r="B35" t="n">
         <v>64.0</v>
       </c>
@@ -1613,9 +510,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
+      <c r="A36"/>
       <c r="B36" t="n">
         <v>70.0</v>
       </c>
@@ -1627,9 +522,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
+      <c r="A37"/>
       <c r="B37" t="n">
         <v>27.0</v>
       </c>
@@ -1641,9 +534,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
+      <c r="A38"/>
       <c r="B38" t="n">
         <v>75.0</v>
       </c>
@@ -1655,9 +546,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
+      <c r="A39"/>
       <c r="B39" t="n">
         <v>0.0</v>
       </c>
@@ -1669,9 +558,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
+      <c r="A40"/>
       <c r="B40" t="n">
         <v>90.0</v>
       </c>
@@ -1683,9 +570,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
+      <c r="A41"/>
       <c r="B41" t="n">
         <v>100.0</v>
       </c>
@@ -1697,9 +582,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
+      <c r="A42"/>
       <c r="B42" t="n">
         <v>100.0</v>
       </c>
@@ -1711,9 +594,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
+      <c r="A43"/>
       <c r="B43" t="n">
         <v>100.0</v>
       </c>
@@ -1725,9 +606,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
+      <c r="A44"/>
       <c r="B44" t="n">
         <v>100.0</v>
       </c>
@@ -1739,9 +618,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
+      <c r="A45"/>
       <c r="B45" t="n">
         <v>100.0</v>
       </c>
@@ -1753,9 +630,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
+      <c r="A46"/>
       <c r="B46" t="n">
         <v>100.0</v>
       </c>
@@ -1767,9 +642,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
+      <c r="A47"/>
       <c r="B47" t="n">
         <v>100.0</v>
       </c>
@@ -1781,9 +654,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
+      <c r="A48"/>
       <c r="B48" t="n">
         <v>100.0</v>
       </c>
@@ -1795,9 +666,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
+      <c r="A49"/>
       <c r="B49" t="n">
         <v>500.0</v>
       </c>
@@ -1809,9 +678,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
+      <c r="A50"/>
       <c r="B50" t="n">
         <v>4000.0</v>
       </c>
@@ -1823,9 +690,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
+      <c r="A51"/>
       <c r="B51" t="n">
         <v>100.0</v>
       </c>
@@ -1837,9 +702,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
+      <c r="A52"/>
       <c r="B52" t="n">
         <v>100.0</v>
       </c>
@@ -1851,9 +714,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
+      <c r="A53"/>
       <c r="B53" t="n">
         <v>100.0</v>
       </c>
@@ -1865,9 +726,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
+      <c r="A54"/>
       <c r="B54" t="n">
         <v>100.0</v>
       </c>
@@ -1879,9 +738,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
-        <v>57</v>
-      </c>
+      <c r="A55"/>
       <c r="B55" t="n">
         <v>0.0</v>
       </c>
@@ -1893,9 +750,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
+      <c r="A56"/>
       <c r="B56" t="n">
         <v>100.0</v>
       </c>
@@ -1907,9 +762,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
+      <c r="A57"/>
       <c r="B57" t="n">
         <v>105.0</v>
       </c>
@@ -1921,9 +774,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
+      <c r="A58"/>
       <c r="B58" t="n">
         <v>120.0</v>
       </c>
@@ -1935,9 +786,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
+      <c r="A59"/>
       <c r="B59" t="n">
         <v>122.0</v>
       </c>
@@ -1949,9 +798,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
+      <c r="A60"/>
       <c r="B60" t="n">
         <v>125.0</v>
       </c>
@@ -1963,9 +810,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s">
-        <v>63</v>
-      </c>
+      <c r="A61"/>
       <c r="B61" t="n">
         <v>0.0</v>
       </c>
@@ -1977,9 +822,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
-        <v>64</v>
-      </c>
+      <c r="A62"/>
       <c r="B62" t="n">
         <v>150.0</v>
       </c>
@@ -1991,9 +834,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
-        <v>65</v>
-      </c>
+      <c r="A63"/>
       <c r="B63" t="n">
         <v>150.0</v>
       </c>
@@ -2005,9 +846,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
-        <v>66</v>
-      </c>
+      <c r="A64"/>
       <c r="B64" t="n">
         <v>0.0</v>
       </c>
@@ -2019,9 +858,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s">
-        <v>67</v>
-      </c>
+      <c r="A65"/>
       <c r="B65" t="n">
         <v>180.0</v>
       </c>
@@ -2033,9 +870,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
-        <v>68</v>
-      </c>
+      <c r="A66"/>
       <c r="B66" t="n">
         <v>180.0</v>
       </c>
@@ -2047,9 +882,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s">
-        <v>69</v>
-      </c>
+      <c r="A67"/>
       <c r="B67" t="n">
         <v>183.0</v>
       </c>
@@ -2061,9 +894,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s">
-        <v>70</v>
-      </c>
+      <c r="A68"/>
       <c r="B68" t="n">
         <v>6438.0</v>
       </c>
@@ -2075,9 +906,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s">
-        <v>71</v>
-      </c>
+      <c r="A69"/>
       <c r="B69" t="n">
         <v>200.0</v>
       </c>
@@ -2089,9 +918,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s">
-        <v>72</v>
-      </c>
+      <c r="A70"/>
       <c r="B70" t="n">
         <v>200.0</v>
       </c>
@@ -2103,9 +930,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="s">
-        <v>73</v>
-      </c>
+      <c r="A71"/>
       <c r="B71" t="n">
         <v>200.0</v>
       </c>
@@ -2117,9 +942,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s">
-        <v>74</v>
-      </c>
+      <c r="A72"/>
       <c r="B72" t="n">
         <v>200.0</v>
       </c>
@@ -2131,9 +954,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s">
-        <v>75</v>
-      </c>
+      <c r="A73"/>
       <c r="B73" t="n">
         <v>200.0</v>
       </c>
@@ -2145,9 +966,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s">
-        <v>76</v>
-      </c>
+      <c r="A74"/>
       <c r="B74" t="n">
         <v>200.0</v>
       </c>
@@ -2159,9 +978,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s">
-        <v>77</v>
-      </c>
+      <c r="A75"/>
       <c r="B75" t="n">
         <v>0.0</v>
       </c>
@@ -2173,9 +990,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="s">
-        <v>78</v>
-      </c>
+      <c r="A76"/>
       <c r="B76" t="n">
         <v>240.0</v>
       </c>
@@ -2187,9 +1002,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="s">
-        <v>79</v>
-      </c>
+      <c r="A77"/>
       <c r="B77" t="n">
         <v>0.0</v>
       </c>
@@ -2201,9 +1014,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="s">
-        <v>80</v>
-      </c>
+      <c r="A78"/>
       <c r="B78" t="n">
         <v>250.0</v>
       </c>
@@ -2215,9 +1026,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="s">
-        <v>81</v>
-      </c>
+      <c r="A79"/>
       <c r="B79" t="n">
         <v>0.0</v>
       </c>
@@ -2229,9 +1038,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="s">
-        <v>82</v>
-      </c>
+      <c r="A80"/>
       <c r="B80" t="n">
         <v>250.0</v>
       </c>
@@ -2243,9 +1050,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="s">
-        <v>83</v>
-      </c>
+      <c r="A81"/>
       <c r="B81" t="n">
         <v>0.0</v>
       </c>
@@ -2257,9 +1062,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s">
-        <v>84</v>
-      </c>
+      <c r="A82"/>
       <c r="B82" t="n">
         <v>250.0</v>
       </c>
@@ -2271,9 +1074,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s">
-        <v>85</v>
-      </c>
+      <c r="A83"/>
       <c r="B83" t="n">
         <v>0.0</v>
       </c>
@@ -2285,9 +1086,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s">
-        <v>86</v>
-      </c>
+      <c r="A84"/>
       <c r="B84" t="n">
         <v>250.0</v>
       </c>
@@ -2299,9 +1098,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s">
-        <v>87</v>
-      </c>
+      <c r="A85"/>
       <c r="B85" t="n">
         <v>250.0</v>
       </c>
@@ -2313,9 +1110,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s">
-        <v>88</v>
-      </c>
+      <c r="A86"/>
       <c r="B86" t="n">
         <v>250.0</v>
       </c>
@@ -2327,9 +1122,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s">
-        <v>89</v>
-      </c>
+      <c r="A87"/>
       <c r="B87" t="n">
         <v>250.0</v>
       </c>
@@ -2341,9 +1134,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s">
-        <v>90</v>
-      </c>
+      <c r="A88"/>
       <c r="B88" t="n">
         <v>0.0</v>
       </c>
@@ -2355,9 +1146,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="s">
-        <v>91</v>
-      </c>
+      <c r="A89"/>
       <c r="B89" t="n">
         <v>0.0</v>
       </c>
@@ -2369,9 +1158,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="s">
-        <v>92</v>
-      </c>
+      <c r="A90"/>
       <c r="B90" t="n">
         <v>0.0</v>
       </c>
@@ -2383,9 +1170,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="s">
-        <v>93</v>
-      </c>
+      <c r="A91"/>
       <c r="B91" t="n">
         <v>250.0</v>
       </c>
@@ -2397,9 +1182,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s">
-        <v>94</v>
-      </c>
+      <c r="A92"/>
       <c r="B92" t="n">
         <v>250.0</v>
       </c>
@@ -2411,9 +1194,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s">
-        <v>95</v>
-      </c>
+      <c r="A93"/>
       <c r="B93" t="n">
         <v>0.0</v>
       </c>
@@ -2425,9 +1206,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="s">
-        <v>96</v>
-      </c>
+      <c r="A94"/>
       <c r="B94" t="n">
         <v>250.0</v>
       </c>
@@ -2439,9 +1218,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="s">
-        <v>97</v>
-      </c>
+      <c r="A95"/>
       <c r="B95" t="n">
         <v>250.0</v>
       </c>
@@ -2453,9 +1230,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="s">
-        <v>98</v>
-      </c>
+      <c r="A96"/>
       <c r="B96" t="n">
         <v>0.0</v>
       </c>
@@ -2467,9 +1242,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="s">
-        <v>99</v>
-      </c>
+      <c r="A97"/>
       <c r="B97" t="n">
         <v>0.0</v>
       </c>
@@ -2481,9 +1254,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s">
-        <v>100</v>
-      </c>
+      <c r="A98"/>
       <c r="B98" t="n">
         <v>300.0</v>
       </c>
@@ -2495,9 +1266,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="s">
-        <v>101</v>
-      </c>
+      <c r="A99"/>
       <c r="B99" t="n">
         <v>300.0</v>
       </c>
@@ -2509,9 +1278,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="s">
-        <v>102</v>
-      </c>
+      <c r="A100"/>
       <c r="B100" t="n">
         <v>0.0</v>
       </c>
@@ -2523,9 +1290,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s">
-        <v>103</v>
-      </c>
+      <c r="A101"/>
       <c r="B101" t="n">
         <v>320.0</v>
       </c>
@@ -2537,9 +1302,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s">
-        <v>104</v>
-      </c>
+      <c r="A102"/>
       <c r="B102" t="n">
         <v>350.0</v>
       </c>
@@ -2551,9 +1314,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s">
-        <v>105</v>
-      </c>
+      <c r="A103"/>
       <c r="B103" t="n">
         <v>350.0</v>
       </c>
@@ -2565,9 +1326,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="s">
-        <v>106</v>
-      </c>
+      <c r="A104"/>
       <c r="B104" t="n">
         <v>0.0</v>
       </c>
@@ -2579,9 +1338,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="s">
-        <v>107</v>
-      </c>
+      <c r="A105"/>
       <c r="B105" t="n">
         <v>110.0</v>
       </c>
@@ -2593,9 +1350,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="s">
-        <v>108</v>
-      </c>
+      <c r="A106"/>
       <c r="B106" t="n">
         <v>387.0</v>
       </c>
@@ -2607,9 +1362,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="s">
-        <v>109</v>
-      </c>
+      <c r="A107"/>
       <c r="B107" t="n">
         <v>0.0</v>
       </c>
@@ -2621,9 +1374,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="s">
-        <v>110</v>
-      </c>
+      <c r="A108"/>
       <c r="B108" t="n">
         <v>400.0</v>
       </c>
@@ -2635,9 +1386,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="s">
-        <v>111</v>
-      </c>
+      <c r="A109"/>
       <c r="B109" t="n">
         <v>425.0</v>
       </c>
@@ -2649,9 +1398,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="s">
-        <v>112</v>
-      </c>
+      <c r="A110"/>
       <c r="B110" t="n">
         <v>490.0</v>
       </c>
@@ -2663,9 +1410,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="s">
-        <v>113</v>
-      </c>
+      <c r="A111"/>
       <c r="B111" t="n">
         <v>450.0</v>
       </c>
@@ -2677,9 +1422,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="s">
-        <v>114</v>
-      </c>
+      <c r="A112"/>
       <c r="B112" t="n">
         <v>450.0</v>
       </c>
@@ -2691,9 +1434,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="s">
-        <v>115</v>
-      </c>
+      <c r="A113"/>
       <c r="B113" t="n">
         <v>0.0</v>
       </c>
@@ -2705,9 +1446,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="s">
-        <v>116</v>
-      </c>
+      <c r="A114"/>
       <c r="B114" t="n">
         <v>450.0</v>
       </c>
@@ -2719,9 +1458,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="s">
-        <v>117</v>
-      </c>
+      <c r="A115"/>
       <c r="B115" t="n">
         <v>450.0</v>
       </c>
@@ -2733,9 +1470,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="s">
-        <v>118</v>
-      </c>
+      <c r="A116"/>
       <c r="B116" t="n">
         <v>484.0</v>
       </c>
@@ -2747,9 +1482,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="s">
-        <v>119</v>
-      </c>
+      <c r="A117"/>
       <c r="B117" t="n">
         <v>490.0</v>
       </c>
@@ -2761,9 +1494,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="s">
-        <v>120</v>
-      </c>
+      <c r="A118"/>
       <c r="B118" t="n">
         <v>500.0</v>
       </c>
@@ -2775,9 +1506,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="s">
-        <v>121</v>
-      </c>
+      <c r="A119"/>
       <c r="B119" t="n">
         <v>500.0</v>
       </c>
@@ -2789,9 +1518,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="s">
-        <v>122</v>
-      </c>
+      <c r="A120"/>
       <c r="B120" t="n">
         <v>500.0</v>
       </c>
@@ -2803,9 +1530,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="s">
-        <v>123</v>
-      </c>
+      <c r="A121"/>
       <c r="B121" t="n">
         <v>0.0</v>
       </c>
@@ -2817,9 +1542,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="s">
-        <v>124</v>
-      </c>
+      <c r="A122"/>
       <c r="B122" t="n">
         <v>0.0</v>
       </c>
@@ -2831,9 +1554,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="s">
-        <v>125</v>
-      </c>
+      <c r="A123"/>
       <c r="B123" t="n">
         <v>500.0</v>
       </c>
@@ -2845,9 +1566,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="s">
-        <v>126</v>
-      </c>
+      <c r="A124"/>
       <c r="B124" t="n">
         <v>0.0</v>
       </c>
@@ -2859,9 +1578,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="s">
-        <v>127</v>
-      </c>
+      <c r="A125"/>
       <c r="B125" t="n">
         <v>500.0</v>
       </c>
@@ -2873,9 +1590,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="s">
-        <v>128</v>
-      </c>
+      <c r="A126"/>
       <c r="B126" t="n">
         <v>0.0</v>
       </c>
@@ -2887,9 +1602,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="s">
-        <v>129</v>
-      </c>
+      <c r="A127"/>
       <c r="B127" t="n">
         <v>500.0</v>
       </c>
@@ -2901,9 +1614,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="s">
-        <v>130</v>
-      </c>
+      <c r="A128"/>
       <c r="B128" t="n">
         <v>500.0</v>
       </c>
@@ -2915,9 +1626,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="s">
-        <v>131</v>
-      </c>
+      <c r="A129"/>
       <c r="B129" t="n">
         <v>500.0</v>
       </c>
@@ -2929,9 +1638,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="s">
-        <v>132</v>
-      </c>
+      <c r="A130"/>
       <c r="B130" t="n">
         <v>0.0</v>
       </c>
@@ -2943,9 +1650,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="s">
-        <v>133</v>
-      </c>
+      <c r="A131"/>
       <c r="B131" t="n">
         <v>0.0</v>
       </c>
@@ -2957,9 +1662,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="s">
-        <v>134</v>
-      </c>
+      <c r="A132"/>
       <c r="B132" t="n">
         <v>500.0</v>
       </c>
@@ -2971,9 +1674,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="s">
-        <v>135</v>
-      </c>
+      <c r="A133"/>
       <c r="B133" t="n">
         <v>550.0</v>
       </c>
@@ -2985,9 +1686,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="s">
-        <v>136</v>
-      </c>
+      <c r="A134"/>
       <c r="B134" t="n">
         <v>0.0</v>
       </c>
@@ -2999,9 +1698,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="s">
-        <v>137</v>
-      </c>
+      <c r="A135"/>
       <c r="B135" t="n">
         <v>350.0</v>
       </c>
@@ -3013,9 +1710,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="s">
-        <v>138</v>
-      </c>
+      <c r="A136"/>
       <c r="B136" t="n">
         <v>150.0</v>
       </c>
@@ -3027,9 +1722,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="s">
-        <v>139</v>
-      </c>
+      <c r="A137"/>
       <c r="B137" t="n">
         <v>0.0</v>
       </c>
@@ -3041,9 +1734,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="s">
-        <v>140</v>
-      </c>
+      <c r="A138"/>
       <c r="B138" t="n">
         <v>0.0</v>
       </c>
@@ -3055,9 +1746,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="s">
-        <v>141</v>
-      </c>
+      <c r="A139"/>
       <c r="B139" t="n">
         <v>0.0</v>
       </c>
@@ -3069,9 +1758,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="s">
-        <v>142</v>
-      </c>
+      <c r="A140"/>
       <c r="B140" t="n">
         <v>800.0</v>
       </c>
@@ -3083,9 +1770,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="s">
-        <v>143</v>
-      </c>
+      <c r="A141"/>
       <c r="B141" t="n">
         <v>0.0</v>
       </c>
@@ -3097,9 +1782,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="s">
-        <v>144</v>
-      </c>
+      <c r="A142"/>
       <c r="B142" t="n">
         <v>10.0</v>
       </c>
@@ -3111,9 +1794,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="s">
-        <v>145</v>
-      </c>
+      <c r="A143"/>
       <c r="B143" t="n">
         <v>955.0</v>
       </c>
@@ -3125,9 +1806,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="s">
-        <v>146</v>
-      </c>
+      <c r="A144"/>
       <c r="B144" t="n">
         <v>1000.0</v>
       </c>
@@ -3139,9 +1818,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="s">
-        <v>147</v>
-      </c>
+      <c r="A145"/>
       <c r="B145" t="n">
         <v>1000.0</v>
       </c>
@@ -3153,9 +1830,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="s">
-        <v>148</v>
-      </c>
+      <c r="A146"/>
       <c r="B146" t="n">
         <v>1000.0</v>
       </c>
@@ -3167,9 +1842,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="s">
-        <v>149</v>
-      </c>
+      <c r="A147"/>
       <c r="B147" t="n">
         <v>1000.0</v>
       </c>
@@ -3181,9 +1854,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="s">
-        <v>150</v>
-      </c>
+      <c r="A148"/>
       <c r="B148" t="n">
         <v>1000.0</v>
       </c>
@@ -3195,9 +1866,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="s">
-        <v>151</v>
-      </c>
+      <c r="A149"/>
       <c r="B149" t="n">
         <v>0.0</v>
       </c>
@@ -3209,9 +1878,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="s">
-        <v>152</v>
-      </c>
+      <c r="A150"/>
       <c r="B150" t="n">
         <v>0.0</v>
       </c>
@@ -3223,9 +1890,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="s">
-        <v>153</v>
-      </c>
+      <c r="A151"/>
       <c r="B151" t="n">
         <v>1100.0</v>
       </c>
@@ -3237,9 +1902,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="s">
-        <v>154</v>
-      </c>
+      <c r="A152"/>
       <c r="B152" t="n">
         <v>1100.0</v>
       </c>
@@ -3251,9 +1914,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="s">
-        <v>155</v>
-      </c>
+      <c r="A153"/>
       <c r="B153" t="n">
         <v>1180.0</v>
       </c>
@@ -3265,9 +1926,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="s">
-        <v>156</v>
-      </c>
+      <c r="A154"/>
       <c r="B154" t="n">
         <v>1322.0</v>
       </c>
@@ -3279,9 +1938,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="s">
-        <v>157</v>
-      </c>
+      <c r="A155"/>
       <c r="B155" t="n">
         <v>0.0</v>
       </c>
@@ -3293,9 +1950,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="s">
-        <v>158</v>
-      </c>
+      <c r="A156"/>
       <c r="B156" t="n">
         <v>0.0</v>
       </c>
@@ -3307,9 +1962,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="s">
-        <v>159</v>
-      </c>
+      <c r="A157"/>
       <c r="B157" t="n">
         <v>0.0</v>
       </c>
@@ -3321,9 +1974,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="s">
-        <v>160</v>
-      </c>
+      <c r="A158"/>
       <c r="B158" t="n">
         <v>7800.0</v>
       </c>
@@ -3335,9 +1986,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="s">
-        <v>161</v>
-      </c>
+      <c r="A159"/>
       <c r="B159" t="n">
         <v>2000.0</v>
       </c>
@@ -3349,9 +1998,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="s">
-        <v>162</v>
-      </c>
+      <c r="A160"/>
       <c r="B160" t="n">
         <v>0.0</v>
       </c>
@@ -3363,9 +2010,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="s">
-        <v>163</v>
-      </c>
+      <c r="A161"/>
       <c r="B161" t="n">
         <v>2307.0</v>
       </c>
@@ -3377,9 +2022,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="s">
-        <v>164</v>
-      </c>
+      <c r="A162"/>
       <c r="B162" t="n">
         <v>0.0</v>
       </c>
@@ -3391,9 +2034,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="s">
-        <v>165</v>
-      </c>
+      <c r="A163"/>
       <c r="B163" t="n">
         <v>2500.0</v>
       </c>
@@ -3405,9 +2046,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="s">
-        <v>166</v>
-      </c>
+      <c r="A164"/>
       <c r="B164" t="n">
         <v>0.0</v>
       </c>
@@ -3419,9 +2058,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="s">
-        <v>167</v>
-      </c>
+      <c r="A165"/>
       <c r="B165" t="n">
         <v>2677.0</v>
       </c>
@@ -3433,9 +2070,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="s">
-        <v>168</v>
-      </c>
+      <c r="A166"/>
       <c r="B166" t="n">
         <v>2777.0</v>
       </c>
@@ -3447,9 +2082,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="s">
-        <v>169</v>
-      </c>
+      <c r="A167"/>
       <c r="B167" t="n">
         <v>3134.0</v>
       </c>
@@ -3461,9 +2094,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="s">
-        <v>170</v>
-      </c>
+      <c r="A168"/>
       <c r="B168" t="n">
         <v>3249.0</v>
       </c>
@@ -3475,9 +2106,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="s">
-        <v>171</v>
-      </c>
+      <c r="A169"/>
       <c r="B169" t="n">
         <v>3502.0</v>
       </c>
@@ -3489,9 +2118,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="s">
-        <v>172</v>
-      </c>
+      <c r="A170"/>
       <c r="B170" t="n">
         <v>3803.0</v>
       </c>
@@ -3503,9 +2130,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="s">
-        <v>173</v>
-      </c>
+      <c r="A171"/>
       <c r="B171" t="n">
         <v>4886.0</v>
       </c>
@@ -3517,9 +2142,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="s">
-        <v>174</v>
-      </c>
+      <c r="A172"/>
       <c r="B172" t="n">
         <v>4964.0</v>
       </c>
@@ -3531,9 +2154,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="s">
-        <v>175</v>
-      </c>
+      <c r="A173"/>
       <c r="B173" t="n">
         <v>5000.0</v>
       </c>
@@ -3545,9 +2166,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="s">
-        <v>176</v>
-      </c>
+      <c r="A174"/>
       <c r="B174" t="n">
         <v>2500.0</v>
       </c>
@@ -3559,9 +2178,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="s">
-        <v>177</v>
-      </c>
+      <c r="A175"/>
       <c r="B175" t="n">
         <v>0.0</v>
       </c>
@@ -3573,9 +2190,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="s">
-        <v>178</v>
-      </c>
+      <c r="A176"/>
       <c r="B176" t="n">
         <v>5000.0</v>
       </c>
@@ -3587,9 +2202,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="s">
-        <v>179</v>
-      </c>
+      <c r="A177"/>
       <c r="B177" t="n">
         <v>5000.0</v>
       </c>
@@ -3601,9 +2214,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="s">
-        <v>180</v>
-      </c>
+      <c r="A178"/>
       <c r="B178" t="n">
         <v>5400.0</v>
       </c>
@@ -3615,9 +2226,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="s">
-        <v>181</v>
-      </c>
+      <c r="A179"/>
       <c r="B179" t="n">
         <v>6647.0</v>
       </c>
@@ -3629,9 +2238,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="s">
-        <v>182</v>
-      </c>
+      <c r="A180"/>
       <c r="B180" t="n">
         <v>6764.0</v>
       </c>
@@ -3643,9 +2250,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="s">
-        <v>183</v>
-      </c>
+      <c r="A181"/>
       <c r="B181" t="n">
         <v>16800.0</v>
       </c>
@@ -3657,9 +2262,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="s">
-        <v>184</v>
-      </c>
+      <c r="A182"/>
       <c r="B182" t="n">
         <v>7363.0</v>
       </c>
@@ -3671,9 +2274,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="s">
-        <v>185</v>
-      </c>
+      <c r="A183"/>
       <c r="B183" t="n">
         <v>7500.0</v>
       </c>
@@ -3685,9 +2286,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="s">
-        <v>186</v>
-      </c>
+      <c r="A184"/>
       <c r="B184" t="n">
         <v>7800.0</v>
       </c>
@@ -3699,9 +2298,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="s">
-        <v>187</v>
-      </c>
+      <c r="A185"/>
       <c r="B185" t="n">
         <v>10000.0</v>
       </c>
@@ -3713,9 +2310,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="s">
-        <v>188</v>
-      </c>
+      <c r="A186"/>
       <c r="B186" t="n">
         <v>93000.0</v>
       </c>
@@ -3727,9 +2322,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="s">
-        <v>189</v>
-      </c>
+      <c r="A187"/>
       <c r="B187" t="n">
         <v>15000.0</v>
       </c>
@@ -3741,9 +2334,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="s">
-        <v>190</v>
-      </c>
+      <c r="A188"/>
       <c r="B188" t="n">
         <v>12943.0</v>
       </c>
@@ -3755,9 +2346,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="s">
-        <v>191</v>
-      </c>
+      <c r="A189"/>
       <c r="B189" t="n">
         <v>13723.0</v>
       </c>
@@ -3769,9 +2358,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="s">
-        <v>192</v>
-      </c>
+      <c r="A190"/>
       <c r="B190" t="n">
         <v>0.0</v>
       </c>
@@ -3783,9 +2370,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="s">
-        <v>193</v>
-      </c>
+      <c r="A191"/>
       <c r="B191" t="n">
         <v>14200.0</v>
       </c>
@@ -3797,9 +2382,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="s">
-        <v>194</v>
-      </c>
+      <c r="A192"/>
       <c r="B192" t="n">
         <v>16000.0</v>
       </c>
@@ -3811,9 +2394,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="s">
-        <v>195</v>
-      </c>
+      <c r="A193"/>
       <c r="B193" t="n">
         <v>17702.0</v>
       </c>
@@ -3825,9 +2406,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="s">
-        <v>196</v>
-      </c>
+      <c r="A194"/>
       <c r="B194" t="n">
         <v>18900.0</v>
       </c>
@@ -3839,9 +2418,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="s">
-        <v>197</v>
-      </c>
+      <c r="A195"/>
       <c r="B195" t="n">
         <v>0.0</v>
       </c>
@@ -3853,9 +2430,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" t="s">
-        <v>198</v>
-      </c>
+      <c r="A196"/>
       <c r="B196" t="n">
         <v>3500.0</v>
       </c>
@@ -3867,9 +2442,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="s">
-        <v>199</v>
-      </c>
+      <c r="A197"/>
       <c r="B197" t="n">
         <v>22500.0</v>
       </c>
@@ -3881,9 +2454,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="s">
-        <v>200</v>
-      </c>
+      <c r="A198"/>
       <c r="B198" t="n">
         <v>25124.0</v>
       </c>
@@ -3895,9 +2466,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="s">
-        <v>201</v>
-      </c>
+      <c r="A199"/>
       <c r="B199" t="n">
         <v>47337.0</v>
       </c>
@@ -3909,9 +2478,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="s">
-        <v>202</v>
-      </c>
+      <c r="A200"/>
       <c r="B200" t="n">
         <v>32000.0</v>
       </c>
@@ -3923,9 +2490,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="s">
-        <v>203</v>
-      </c>
+      <c r="A201"/>
       <c r="B201" t="n">
         <v>27000.0</v>
       </c>
@@ -3937,9 +2502,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="s">
-        <v>204</v>
-      </c>
+      <c r="A202"/>
       <c r="B202" t="n">
         <v>31200.0</v>
       </c>
@@ -3951,9 +2514,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="s">
-        <v>205</v>
-      </c>
+      <c r="A203"/>
       <c r="B203" t="n">
         <v>33600.0</v>
       </c>
@@ -3965,9 +2526,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="s">
-        <v>206</v>
-      </c>
+      <c r="A204"/>
       <c r="B204" t="n">
         <v>35625.0</v>
       </c>
@@ -3979,9 +2538,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="s">
-        <v>207</v>
-      </c>
+      <c r="A205"/>
       <c r="B205" t="n">
         <v>45922.0</v>
       </c>
@@ -3993,9 +2550,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="s">
-        <v>208</v>
-      </c>
+      <c r="A206"/>
       <c r="B206" t="n">
         <v>38962.0</v>
       </c>
@@ -4007,9 +2562,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="s">
-        <v>209</v>
-      </c>
+      <c r="A207"/>
       <c r="B207" t="n">
         <v>40800.0</v>
       </c>
@@ -4021,9 +2574,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" t="s">
-        <v>210</v>
-      </c>
+      <c r="A208"/>
       <c r="B208" t="n">
         <v>44055.0</v>
       </c>
@@ -4035,9 +2586,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" t="s">
-        <v>211</v>
-      </c>
+      <c r="A209"/>
       <c r="B209" t="n">
         <v>44268.0</v>
       </c>
@@ -4049,9 +2598,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" t="s">
-        <v>212</v>
-      </c>
+      <c r="A210"/>
       <c r="B210" t="n">
         <v>25300.0</v>
       </c>
@@ -4063,9 +2610,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" t="s">
-        <v>213</v>
-      </c>
+      <c r="A211"/>
       <c r="B211" t="n">
         <v>50000.0</v>
       </c>
@@ -4077,9 +2622,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" t="s">
-        <v>214</v>
-      </c>
+      <c r="A212"/>
       <c r="B212" t="n">
         <v>55657.0</v>
       </c>
@@ -4091,9 +2634,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" t="s">
-        <v>215</v>
-      </c>
+      <c r="A213"/>
       <c r="B213" t="n">
         <v>60000.0</v>
       </c>
@@ -4105,9 +2646,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" t="s">
-        <v>216</v>
-      </c>
+      <c r="A214"/>
       <c r="B214" t="n">
         <v>73613.0</v>
       </c>
@@ -4119,9 +2658,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" t="s">
-        <v>217</v>
-      </c>
+      <c r="A215"/>
       <c r="B215" t="n">
         <v>64450.0</v>
       </c>
@@ -4133,9 +2670,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" t="s">
-        <v>218</v>
-      </c>
+      <c r="A216"/>
       <c r="B216" t="n">
         <v>78000.0</v>
       </c>
@@ -4147,9 +2682,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="s">
-        <v>219</v>
-      </c>
+      <c r="A217"/>
       <c r="B217" t="n">
         <v>61079.0</v>
       </c>
@@ -4161,9 +2694,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" t="s">
-        <v>220</v>
-      </c>
+      <c r="A218"/>
       <c r="B218" t="n">
         <v>0.0</v>
       </c>
@@ -4175,9 +2706,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="s">
-        <v>221</v>
-      </c>
+      <c r="A219"/>
       <c r="B219" t="n">
         <v>8207.0</v>
       </c>
@@ -4189,9 +2718,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="s">
-        <v>222</v>
-      </c>
+      <c r="A220"/>
       <c r="B220" t="n">
         <v>137500.0</v>
       </c>
@@ -4203,9 +2730,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" t="s">
-        <v>223</v>
-      </c>
+      <c r="A221"/>
       <c r="B221" t="n">
         <v>92803.0</v>
       </c>
@@ -4217,9 +2742,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="s">
-        <v>224</v>
-      </c>
+      <c r="A222"/>
       <c r="B222" t="n">
         <v>0.0</v>
       </c>
@@ -4231,9 +2754,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" t="s">
-        <v>225</v>
-      </c>
+      <c r="A223"/>
       <c r="B223" t="n">
         <v>99089.0</v>
       </c>
@@ -4245,9 +2766,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" t="s">
-        <v>226</v>
-      </c>
+      <c r="A224"/>
       <c r="B224" t="n">
         <v>62928.0</v>
       </c>
@@ -4259,9 +2778,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" t="s">
-        <v>227</v>
-      </c>
+      <c r="A225"/>
       <c r="B225" t="n">
         <v>106173.0</v>
       </c>
@@ -4273,9 +2790,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" t="s">
-        <v>228</v>
-      </c>
+      <c r="A226"/>
       <c r="B226" t="n">
         <v>113006.0</v>
       </c>
@@ -4287,9 +2802,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" t="s">
-        <v>229</v>
-      </c>
+      <c r="A227"/>
       <c r="B227" t="n">
         <v>115504.0</v>
       </c>
@@ -4301,9 +2814,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" t="s">
-        <v>230</v>
-      </c>
+      <c r="A228"/>
       <c r="B228" t="n">
         <v>117577.0</v>
       </c>
@@ -4315,9 +2826,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" t="s">
-        <v>231</v>
-      </c>
+      <c r="A229"/>
       <c r="B229" t="n">
         <v>0.0</v>
       </c>
@@ -4329,9 +2838,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="s">
-        <v>232</v>
-      </c>
+      <c r="A230"/>
       <c r="B230" t="n">
         <v>126629.0</v>
       </c>
@@ -4343,9 +2850,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="s">
-        <v>233</v>
-      </c>
+      <c r="A231"/>
       <c r="B231" t="n">
         <v>0.0</v>
       </c>
@@ -4357,9 +2862,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" t="s">
-        <v>234</v>
-      </c>
+      <c r="A232"/>
       <c r="B232" t="n">
         <v>150000.0</v>
       </c>
@@ -4371,9 +2874,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" t="s">
-        <v>235</v>
-      </c>
+      <c r="A233"/>
       <c r="B233" t="n">
         <v>713781.0</v>
       </c>
@@ -4385,9 +2886,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" t="s">
-        <v>236</v>
-      </c>
+      <c r="A234"/>
       <c r="B234" t="n">
         <v>168750.0</v>
       </c>
@@ -4399,9 +2898,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" t="s">
-        <v>237</v>
-      </c>
+      <c r="A235"/>
       <c r="B235" t="n">
         <v>172343.0</v>
       </c>
@@ -4413,9 +2910,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="s">
-        <v>238</v>
-      </c>
+      <c r="A236"/>
       <c r="B236" t="n">
         <v>32402.0</v>
       </c>
@@ -4427,9 +2922,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" t="s">
-        <v>239</v>
-      </c>
+      <c r="A237"/>
       <c r="B237" t="n">
         <v>0.0</v>
       </c>
@@ -4441,9 +2934,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="s">
-        <v>240</v>
-      </c>
+      <c r="A238"/>
       <c r="B238" t="n">
         <v>199720.0</v>
       </c>
@@ -4455,9 +2946,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" t="s">
-        <v>241</v>
-      </c>
+      <c r="A239"/>
       <c r="B239" t="n">
         <v>200000.0</v>
       </c>
@@ -4469,9 +2958,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" t="s">
-        <v>242</v>
-      </c>
+      <c r="A240"/>
       <c r="B240" t="n">
         <v>203481.0</v>
       </c>
@@ -4483,9 +2970,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" t="s">
-        <v>243</v>
-      </c>
+      <c r="A241"/>
       <c r="B241" t="n">
         <v>52516.0</v>
       </c>
@@ -4497,9 +2982,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" t="s">
-        <v>244</v>
-      </c>
+      <c r="A242"/>
       <c r="B242" t="n">
         <v>213278.0</v>
       </c>
@@ -4511,9 +2994,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" t="s">
-        <v>245</v>
-      </c>
+      <c r="A243"/>
       <c r="B243" t="n">
         <v>240000.0</v>
       </c>
@@ -4525,9 +3006,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" t="s">
-        <v>246</v>
-      </c>
+      <c r="A244"/>
       <c r="B244" t="n">
         <v>251601.0</v>
       </c>
@@ -4539,9 +3018,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" t="s">
-        <v>247</v>
-      </c>
+      <c r="A245"/>
       <c r="B245" t="n">
         <v>655000.0</v>
       </c>
@@ -4553,9 +3030,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="s">
-        <v>248</v>
-      </c>
+      <c r="A246"/>
       <c r="B246" t="n">
         <v>269480.0</v>
       </c>
@@ -4567,9 +3042,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" t="s">
-        <v>249</v>
-      </c>
+      <c r="A247"/>
       <c r="B247" t="n">
         <v>272925.0</v>
       </c>
@@ -4581,9 +3054,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" t="s">
-        <v>250</v>
-      </c>
+      <c r="A248"/>
       <c r="B248" t="n">
         <v>309000.0</v>
       </c>
@@ -4595,9 +3066,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" t="s">
-        <v>251</v>
-      </c>
+      <c r="A249"/>
       <c r="B249" t="n">
         <v>312956.0</v>
       </c>
@@ -4609,9 +3078,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" t="s">
-        <v>252</v>
-      </c>
+      <c r="A250"/>
       <c r="B250" t="n">
         <v>324803.0</v>
       </c>
@@ -4623,9 +3090,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="s">
-        <v>253</v>
-      </c>
+      <c r="A251"/>
       <c r="B251" t="n">
         <v>354789.0</v>
       </c>
@@ -4637,9 +3102,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" t="s">
-        <v>254</v>
-      </c>
+      <c r="A252"/>
       <c r="B252" t="n">
         <v>385148.0</v>
       </c>
@@ -4651,9 +3114,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" t="s">
-        <v>255</v>
-      </c>
+      <c r="A253"/>
       <c r="B253" t="n">
         <v>802000.0</v>
       </c>
@@ -4665,9 +3126,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" t="s">
-        <v>256</v>
-      </c>
+      <c r="A254"/>
       <c r="B254" t="n">
         <v>441144.0</v>
       </c>
@@ -4679,9 +3138,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" t="s">
-        <v>257</v>
-      </c>
+      <c r="A255"/>
       <c r="B255" t="n">
         <v>312420.00001</v>
       </c>
@@ -4693,9 +3150,7 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" t="s">
-        <v>258</v>
-      </c>
+      <c r="A256"/>
       <c r="B256" t="n">
         <v>1500000.0</v>
       </c>
@@ -4707,9 +3162,7 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" t="s">
-        <v>259</v>
-      </c>
+      <c r="A257"/>
       <c r="B257" t="n">
         <v>500000.0</v>
       </c>
@@ -4721,9 +3174,7 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" t="s">
-        <v>260</v>
-      </c>
+      <c r="A258"/>
       <c r="B258" t="n">
         <v>437885.0</v>
       </c>
@@ -4735,9 +3186,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" t="s">
-        <v>261</v>
-      </c>
+      <c r="A259"/>
       <c r="B259" t="n">
         <v>0.0</v>
       </c>
@@ -4749,9 +3198,7 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" t="s">
-        <v>262</v>
-      </c>
+      <c r="A260"/>
       <c r="B260" t="n">
         <v>476527.0</v>
       </c>
@@ -4763,9 +3210,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" t="s">
-        <v>263</v>
-      </c>
+      <c r="A261"/>
       <c r="B261" t="n">
         <v>533344.0</v>
       </c>
@@ -4777,9 +3222,7 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" t="s">
-        <v>264</v>
-      </c>
+      <c r="A262"/>
       <c r="B262" t="n">
         <v>71916.0</v>
       </c>
@@ -4791,9 +3234,7 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" t="s">
-        <v>265</v>
-      </c>
+      <c r="A263"/>
       <c r="B263" t="n">
         <v>541741.0</v>
       </c>
@@ -4805,9 +3246,7 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" t="s">
-        <v>266</v>
-      </c>
+      <c r="A264"/>
       <c r="B264" t="n">
         <v>582400.0</v>
       </c>
@@ -4819,9 +3258,7 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" t="s">
-        <v>267</v>
-      </c>
+      <c r="A265"/>
       <c r="B265" t="n">
         <v>562880.0</v>
       </c>
@@ -4833,9 +3270,7 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" t="s">
-        <v>268</v>
-      </c>
+      <c r="A266"/>
       <c r="B266" t="n">
         <v>637349.0</v>
       </c>
@@ -4847,9 +3282,7 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" t="s">
-        <v>269</v>
-      </c>
+      <c r="A267"/>
       <c r="B267" t="n">
         <v>1114342.0</v>
       </c>
@@ -4861,9 +3294,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" t="s">
-        <v>270</v>
-      </c>
+      <c r="A268"/>
       <c r="B268" t="n">
         <v>813845.0</v>
       </c>
@@ -4875,9 +3306,7 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" t="s">
-        <v>271</v>
-      </c>
+      <c r="A269"/>
       <c r="B269" t="n">
         <v>468191.0</v>
       </c>
@@ -4889,9 +3318,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" t="s">
-        <v>272</v>
-      </c>
+      <c r="A270"/>
       <c r="B270" t="n">
         <v>894473.0</v>
       </c>
@@ -4903,9 +3330,7 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" t="s">
-        <v>273</v>
-      </c>
+      <c r="A271"/>
       <c r="B271" t="n">
         <v>1100000.0</v>
       </c>
@@ -4917,9 +3342,7 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" t="s">
-        <v>274</v>
-      </c>
+      <c r="A272"/>
       <c r="B272" t="n">
         <v>947174.0</v>
       </c>
@@ -4931,9 +3354,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" t="s">
-        <v>275</v>
-      </c>
+      <c r="A273"/>
       <c r="B273" t="n">
         <v>854674.0</v>
       </c>
@@ -4945,9 +3366,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" t="s">
-        <v>276</v>
-      </c>
+      <c r="A274"/>
       <c r="B274" t="n">
         <v>0.0</v>
       </c>
@@ -4959,9 +3378,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" t="s">
-        <v>277</v>
-      </c>
+      <c r="A275"/>
       <c r="B275" t="n">
         <v>837246.0</v>
       </c>
@@ -4973,9 +3390,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" t="s">
-        <v>278</v>
-      </c>
+      <c r="A276"/>
       <c r="B276" t="n">
         <v>981200.0</v>
       </c>
@@ -4987,9 +3402,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="s">
-        <v>279</v>
-      </c>
+      <c r="A277"/>
       <c r="B277" t="n">
         <v>1038448.0</v>
       </c>
@@ -5001,9 +3414,7 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" t="s">
-        <v>280</v>
-      </c>
+      <c r="A278"/>
       <c r="B278" t="n">
         <v>0.0</v>
       </c>
@@ -5015,9 +3426,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="s">
-        <v>281</v>
-      </c>
+      <c r="A279"/>
       <c r="B279" t="n">
         <v>1004158.0</v>
       </c>
@@ -5029,9 +3438,7 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" t="s">
-        <v>282</v>
-      </c>
+      <c r="A280"/>
       <c r="B280" t="n">
         <v>1078000.0</v>
       </c>
@@ -5043,9 +3450,7 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" t="s">
-        <v>283</v>
-      </c>
+      <c r="A281"/>
       <c r="B281" t="n">
         <v>1092000.0</v>
       </c>
@@ -5057,9 +3462,7 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" t="s">
-        <v>284</v>
-      </c>
+      <c r="A282"/>
       <c r="B282" t="n">
         <v>1110000.0</v>
       </c>
@@ -5071,9 +3474,7 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" t="s">
-        <v>285</v>
-      </c>
+      <c r="A283"/>
       <c r="B283" t="n">
         <v>1115086.0</v>
       </c>
@@ -5085,9 +3486,7 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" t="s">
-        <v>286</v>
-      </c>
+      <c r="A284"/>
       <c r="B284" t="n">
         <v>1022166.0</v>
       </c>
@@ -5099,9 +3498,7 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" t="s">
-        <v>287</v>
-      </c>
+      <c r="A285"/>
       <c r="B285" t="n">
         <v>996649.0</v>
       </c>
@@ -5113,9 +3510,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" t="s">
-        <v>288</v>
-      </c>
+      <c r="A286"/>
       <c r="B286" t="n">
         <v>137772.0</v>
       </c>
@@ -5127,9 +3522,7 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" t="s">
-        <v>289</v>
-      </c>
+      <c r="A287"/>
       <c r="B287" t="n">
         <v>892958.0</v>
       </c>
@@ -5141,9 +3534,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" t="s">
-        <v>290</v>
-      </c>
+      <c r="A288"/>
       <c r="B288" t="n">
         <v>1286057.0</v>
       </c>
@@ -5155,9 +3546,7 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" t="s">
-        <v>291</v>
-      </c>
+      <c r="A289"/>
       <c r="B289" t="n">
         <v>1271973.0</v>
       </c>
@@ -5169,9 +3558,7 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" t="s">
-        <v>292</v>
-      </c>
+      <c r="A290"/>
       <c r="B290" t="n">
         <v>1224740.0</v>
       </c>
@@ -5183,9 +3570,7 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" t="s">
-        <v>293</v>
-      </c>
+      <c r="A291"/>
       <c r="B291" t="n">
         <v>1331084.0</v>
       </c>
@@ -5197,9 +3582,7 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" t="s">
-        <v>294</v>
-      </c>
+      <c r="A292"/>
       <c r="B292" t="n">
         <v>1501541.0</v>
       </c>
@@ -5211,9 +3594,7 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" t="s">
-        <v>295</v>
-      </c>
+      <c r="A293"/>
       <c r="B293" t="n">
         <v>1508924.0</v>
       </c>
@@ -5225,9 +3606,7 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" t="s">
-        <v>296</v>
-      </c>
+      <c r="A294"/>
       <c r="B294" t="n">
         <v>1587982.0</v>
       </c>
@@ -5239,9 +3618,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" t="s">
-        <v>297</v>
-      </c>
+      <c r="A295"/>
       <c r="B295" t="n">
         <v>1651500.0</v>
       </c>
@@ -5253,9 +3630,7 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" t="s">
-        <v>298</v>
-      </c>
+      <c r="A296"/>
       <c r="B296" t="n">
         <v>1683662.0</v>
       </c>
@@ -5267,9 +3642,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" t="s">
-        <v>299</v>
-      </c>
+      <c r="A297"/>
       <c r="B297" t="n">
         <v>1712141.0</v>
       </c>
@@ -5281,9 +3654,7 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" t="s">
-        <v>300</v>
-      </c>
+      <c r="A298"/>
       <c r="B298" t="n">
         <v>1022360.0</v>
       </c>
@@ -5295,9 +3666,7 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" t="s">
-        <v>301</v>
-      </c>
+      <c r="A299"/>
       <c r="B299" t="n">
         <v>1342615.0</v>
       </c>
@@ -5309,9 +3678,7 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" t="s">
-        <v>302</v>
-      </c>
+      <c r="A300"/>
       <c r="B300" t="n">
         <v>1887765.0</v>
       </c>
@@ -5323,9 +3690,7 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" t="s">
-        <v>303</v>
-      </c>
+      <c r="A301"/>
       <c r="B301" t="n">
         <v>2000830.0</v>
       </c>
@@ -5337,9 +3702,7 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" t="s">
-        <v>304</v>
-      </c>
+      <c r="A302"/>
       <c r="B302" t="n">
         <v>2010080.0</v>
       </c>
@@ -5351,9 +3714,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" t="s">
-        <v>305</v>
-      </c>
+      <c r="A303"/>
       <c r="B303" t="n">
         <v>2700000.0</v>
       </c>
@@ -5365,9 +3726,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" t="s">
-        <v>306</v>
-      </c>
+      <c r="A304"/>
       <c r="B304" t="n">
         <v>1412560.0</v>
       </c>
@@ -5379,9 +3738,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" t="s">
-        <v>307</v>
-      </c>
+      <c r="A305"/>
       <c r="B305" t="n">
         <v>2171184.0</v>
       </c>
@@ -5393,9 +3750,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" t="s">
-        <v>308</v>
-      </c>
+      <c r="A306"/>
       <c r="B306" t="n">
         <v>754620.0</v>
       </c>
@@ -5407,9 +3762,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" t="s">
-        <v>309</v>
-      </c>
+      <c r="A307"/>
       <c r="B307" t="n">
         <v>1500171.0</v>
       </c>
@@ -5421,9 +3774,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" t="s">
-        <v>310</v>
-      </c>
+      <c r="A308"/>
       <c r="B308" t="n">
         <v>3410705.0</v>
       </c>
@@ -5435,9 +3786,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" t="s">
-        <v>311</v>
-      </c>
+      <c r="A309"/>
       <c r="B309" t="n">
         <v>5618482.0</v>
       </c>
@@ -5449,9 +3798,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" t="s">
-        <v>312</v>
-      </c>
+      <c r="A310"/>
       <c r="B310" t="n">
         <v>2555038.0</v>
       </c>
@@ -5463,9 +3810,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" t="s">
-        <v>313</v>
-      </c>
+      <c r="A311"/>
       <c r="B311" t="n">
         <v>2350000.0</v>
       </c>
@@ -5477,9 +3822,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" t="s">
-        <v>314</v>
-      </c>
+      <c r="A312"/>
       <c r="B312" t="n">
         <v>2745084.0</v>
       </c>
@@ -5491,9 +3834,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" t="s">
-        <v>315</v>
-      </c>
+      <c r="A313"/>
       <c r="B313" t="n">
         <v>2117090.0</v>
       </c>
@@ -5505,9 +3846,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" t="s">
-        <v>316</v>
-      </c>
+      <c r="A314"/>
       <c r="B314" t="n">
         <v>3076959.0</v>
       </c>
@@ -5519,9 +3858,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" t="s">
-        <v>317</v>
-      </c>
+      <c r="A315"/>
       <c r="B315" t="n">
         <v>3283000.0</v>
       </c>
@@ -5533,9 +3870,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" t="s">
-        <v>318</v>
-      </c>
+      <c r="A316"/>
       <c r="B316" t="n">
         <v>3374626.0</v>
       </c>
@@ -5547,9 +3882,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" t="s">
-        <v>319</v>
-      </c>
+      <c r="A317"/>
       <c r="B317" t="n">
         <v>3940822.0</v>
       </c>
@@ -5561,9 +3894,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" t="s">
-        <v>320</v>
-      </c>
+      <c r="A318"/>
       <c r="B318" t="n">
         <v>3994796.0</v>
       </c>
@@ -5575,9 +3906,7 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" t="s">
-        <v>321</v>
-      </c>
+      <c r="A319"/>
       <c r="B319" t="n">
         <v>4306839.0</v>
       </c>
@@ -5589,9 +3918,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" t="s">
-        <v>322</v>
-      </c>
+      <c r="A320"/>
       <c r="B320" t="n">
         <v>4471966.0</v>
       </c>
@@ -5603,9 +3930,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" t="s">
-        <v>323</v>
-      </c>
+      <c r="A321"/>
       <c r="B321" t="n">
         <v>3810000.0</v>
       </c>
@@ -5617,9 +3942,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" t="s">
-        <v>324</v>
-      </c>
+      <c r="A322"/>
       <c r="B322" t="n">
         <v>4526797.0</v>
       </c>
@@ -5631,9 +3954,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" t="s">
-        <v>325</v>
-      </c>
+      <c r="A323"/>
       <c r="B323" t="n">
         <v>4909105.0</v>
       </c>
@@ -5645,9 +3966,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" t="s">
-        <v>326</v>
-      </c>
+      <c r="A324"/>
       <c r="B324" t="n">
         <v>5567233.0</v>
       </c>
@@ -5659,9 +3978,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" t="s">
-        <v>327</v>
-      </c>
+      <c r="A325"/>
       <c r="B325" t="n">
         <v>6282339.0</v>
       </c>
@@ -5673,9 +3990,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" t="s">
-        <v>328</v>
-      </c>
+      <c r="A326"/>
       <c r="B326" t="n">
         <v>6367931.0</v>
       </c>
@@ -5687,9 +4002,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" t="s">
-        <v>329</v>
-      </c>
+      <c r="A327"/>
       <c r="B327" t="n">
         <v>7178255.0</v>
       </c>
@@ -5701,9 +4014,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" t="s">
-        <v>330</v>
-      </c>
+      <c r="A328"/>
       <c r="B328" t="n">
         <v>6967747.0</v>
       </c>
@@ -5715,9 +4026,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" t="s">
-        <v>331</v>
-      </c>
+      <c r="A329"/>
       <c r="B329" t="n">
         <v>7334260.0</v>
       </c>
@@ -5729,9 +4038,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" t="s">
-        <v>332</v>
-      </c>
+      <c r="A330"/>
       <c r="B330" t="n">
         <v>1.0260929E7</v>
       </c>
@@ -5743,9 +4050,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" t="s">
-        <v>333</v>
-      </c>
+      <c r="A331"/>
       <c r="B331" t="n">
         <v>1.1712098E7</v>
       </c>
@@ -5757,9 +4062,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" t="s">
-        <v>334</v>
-      </c>
+      <c r="A332"/>
       <c r="B332" t="n">
         <v>1.0972647E7</v>
       </c>
@@ -5771,9 +4074,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" t="s">
-        <v>335</v>
-      </c>
+      <c r="A333"/>
       <c r="B333" t="n">
         <v>1.3670101E7</v>
       </c>
@@ -5785,9 +4086,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" t="s">
-        <v>336</v>
-      </c>
+      <c r="A334"/>
       <c r="B334" t="n">
         <v>1.6749158E7</v>
       </c>
@@ -5799,9 +4098,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" t="s">
-        <v>337</v>
-      </c>
+      <c r="A335"/>
       <c r="B335" t="n">
         <v>1.1728269E7</v>
       </c>
@@ -5813,9 +4110,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" t="s">
-        <v>338</v>
-      </c>
+      <c r="A336"/>
       <c r="B336" t="n">
         <v>1.6953357E7</v>
       </c>
@@ -5827,9 +4122,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" t="s">
-        <v>339</v>
-      </c>
+      <c r="A337"/>
       <c r="B337" t="n">
         <v>1.3652644E7</v>
       </c>
@@ -5841,9 +4134,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" t="s">
-        <v>340</v>
-      </c>
+      <c r="A338"/>
       <c r="B338" t="n">
         <v>1.5922045E7</v>
       </c>
@@ -5855,9 +4146,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" t="s">
-        <v>341</v>
-      </c>
+      <c r="A339"/>
       <c r="B339" t="n">
         <v>1.8141273E7</v>
       </c>
@@ -5869,9 +4158,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" t="s">
-        <v>342</v>
-      </c>
+      <c r="A340"/>
       <c r="B340" t="n">
         <v>2.3254137E7</v>
       </c>
@@ -5883,9 +4170,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" t="s">
-        <v>343</v>
-      </c>
+      <c r="A341"/>
       <c r="B341" t="n">
         <v>2.4919924E7</v>
       </c>
@@ -5897,9 +4182,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" t="s">
-        <v>344</v>
-      </c>
+      <c r="A342"/>
       <c r="B342" t="n">
         <v>2.7462416E7</v>
       </c>
@@ -5911,9 +4194,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" t="s">
-        <v>345</v>
-      </c>
+      <c r="A343"/>
       <c r="B343" t="n">
         <v>3.3960606E7</v>
       </c>
@@ -5925,9 +4206,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" t="s">
-        <v>346</v>
-      </c>
+      <c r="A344"/>
       <c r="B344" t="n">
         <v>3.9833562E7</v>
       </c>
@@ -5939,9 +4218,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" t="s">
-        <v>347</v>
-      </c>
+      <c r="A345"/>
       <c r="B345" t="n">
         <v>1.1547071E7</v>
       </c>
@@ -5953,9 +4230,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" t="s">
-        <v>348</v>
-      </c>
+      <c r="A346"/>
       <c r="B346" t="n">
         <v>4.0493578E7</v>
       </c>

</xml_diff>